<commit_message>
updated results from manual extraction
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkleinlein/Documents/Uni Konstanz/Masterarbeit/Lobby_Synchronozation/among-us-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639301CD-1D78-164A-95A8-E80AF3E9C6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEAAE4A-DA44-1449-98AE-11A049BA24A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" firstSheet="19" activeTab="23" xr2:uid="{9950DF6A-BFE9-1641-98C5-27CAF655A960}"/>
+    <workbookView xWindow="48100" yWindow="3560" windowWidth="28940" windowHeight="16380" firstSheet="15" activeTab="15" xr2:uid="{9950DF6A-BFE9-1641-98C5-27CAF655A960}"/>
   </bookViews>
   <sheets>
     <sheet name="2022-01-25_S1" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="240">
   <si>
     <t>No srt file</t>
   </si>
@@ -1454,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6BBB2A1-7DE6-374B-9B51-A550908847E9}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1575,6 +1575,28 @@
       </c>
       <c r="J7" s="2">
         <v>0.12208333333333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.1006712962962963</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.10765046296296295</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.13614583333333333</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.14758101851851851</v>
       </c>
     </row>
   </sheetData>
@@ -2054,10 +2076,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D77D5D-5E10-9244-A0F6-70CA1A4DB0DD}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2194,6 +2216,17 @@
         <v>0.10979166666666666</v>
       </c>
     </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>4.6087962962962963E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <v>5.1458333333333328E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2201,10 +2234,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CBFEB-58BD-FB4A-984A-6B2B6C69355D}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2283,6 +2316,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="C3" s="4"/>
       <c r="H3">
         <v>2</v>
       </c>
@@ -2323,7 +2357,7 @@
         <v>2.6041666666666665E-3</v>
       </c>
       <c r="J6" s="2">
-        <v>1.2638888888888889E-2</v>
+        <v>2.6041666666666665E-3</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -2390,6 +2424,17 @@
       </c>
       <c r="J12" s="2">
         <v>0.1245949074074074</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="I13" s="2">
+        <v>5.693287037037037E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <v>6.2812499999999993E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2485,10 +2530,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C9402D-A326-7D4E-9CD8-1B9A422D464B}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2584,6 +2629,28 @@
       </c>
       <c r="J5" s="2">
         <v>5.4918981481481478E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2">
+        <v>6.3865740740740737E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>6.8993055555555557E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="2">
+        <v>9.1539351851851858E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>9.5335648148148155E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3791,7 +3858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF7051A-4CAD-7140-9542-2B88FBBB228E}">
   <dimension ref="A1:D170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -6375,10 +6442,10 @@
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56688B2-CB9C-2643-B2C2-FF72E00B094E}">
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8769,6 +8836,132 @@
         <v>0.10857638888888889</v>
       </c>
     </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>128</v>
+      </c>
+      <c r="B171">
+        <v>11</v>
+      </c>
+      <c r="C171" s="2">
+        <v>6.3865740740740737E-2</v>
+      </c>
+      <c r="D171" s="2">
+        <v>6.8993055555555557E-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>128</v>
+      </c>
+      <c r="B172">
+        <v>15</v>
+      </c>
+      <c r="C172" s="2">
+        <v>9.1539351851851858E-2</v>
+      </c>
+      <c r="D172" s="2">
+        <v>9.5335648148148155E-2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>122</v>
+      </c>
+      <c r="B173">
+        <v>13</v>
+      </c>
+      <c r="C173" s="2">
+        <v>5.693287037037037E-2</v>
+      </c>
+      <c r="D173" s="2">
+        <v>6.2812499999999993E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>144</v>
+      </c>
+      <c r="B174">
+        <v>17</v>
+      </c>
+      <c r="C174" s="2">
+        <v>0.10886574074074074</v>
+      </c>
+      <c r="D174" s="2">
+        <v>0.11337962962962962</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>93</v>
+      </c>
+      <c r="B175">
+        <v>15</v>
+      </c>
+      <c r="C175" s="2">
+        <v>0.1006712962962963</v>
+      </c>
+      <c r="D175" s="2">
+        <v>0.10765046296296295</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>93</v>
+      </c>
+      <c r="B176">
+        <v>20</v>
+      </c>
+      <c r="C176" s="2">
+        <v>0.13614583333333333</v>
+      </c>
+      <c r="D176" s="2">
+        <v>0.14758101851851851</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>225</v>
+      </c>
+      <c r="B177">
+        <v>18</v>
+      </c>
+      <c r="C177" s="2">
+        <v>9.9652777777777771E-2</v>
+      </c>
+      <c r="D177" s="2">
+        <v>0.10324074074074074</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>114</v>
+      </c>
+      <c r="B178">
+        <v>7</v>
+      </c>
+      <c r="C178" s="2">
+        <v>4.6087962962962963E-2</v>
+      </c>
+      <c r="D178" s="2">
+        <v>5.1458333333333328E-2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>148</v>
+      </c>
+      <c r="B179">
+        <v>12</v>
+      </c>
+      <c r="C179" s="2">
+        <v>9.1585648148148138E-2</v>
+      </c>
+      <c r="D179" s="2">
+        <v>9.7118055555555569E-2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8777,10 +8970,10 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51566731-C169-0D46-AE8C-4651BD7D140D}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8945,6 +9138,17 @@
         <v>0.12019675925925927</v>
       </c>
     </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.10886574074074074</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.11337962962962962</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8952,10 +9156,10 @@
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{755E1020-7197-5E4F-B79B-FB5C8B1D34CB}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9093,6 +9297,17 @@
       </c>
       <c r="J6" s="2">
         <v>0.11709490740740741</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7" s="2">
+        <v>9.1585648148148138E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>9.7118055555555569E-2</v>
       </c>
     </row>
   </sheetData>
@@ -9764,10 +9979,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC3B62F-6066-7945-A10E-BBF762BE061A}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9928,6 +10143,17 @@
       </c>
       <c r="J11" s="2">
         <v>0.10584490740740742</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>18</v>
+      </c>
+      <c r="I12" s="2">
+        <v>9.9652777777777771E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.10324074074074074</v>
       </c>
     </row>
   </sheetData>

</xml_diff>